<commit_message>
Add z and tno variable to program
</commit_message>
<xml_diff>
--- a/docs/RealTimeVariables.xlsx
+++ b/docs/RealTimeVariables.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="147">
   <si>
     <t>pf</t>
   </si>
@@ -439,6 +439,27 @@
   </si>
   <si>
     <t>ورود یا خروج پول حقیقی</t>
+  </si>
+  <si>
+    <t>tno</t>
+  </si>
+  <si>
+    <t>tvol</t>
+  </si>
+  <si>
+    <t>tval</t>
+  </si>
+  <si>
+    <t>تعداد معاملات</t>
+  </si>
+  <si>
+    <t>ارزش معاملات</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>تعداد سهام</t>
   </si>
 </sst>
 </file>
@@ -785,10 +806,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B70"/>
+  <dimension ref="A1:B74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A1048554" workbookViewId="0">
+      <selection activeCell="C1048576" sqref="C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,433 +948,465 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="B17" t="s">
-        <v>80</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>141</v>
       </c>
       <c r="B18" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>142</v>
       </c>
       <c r="B19" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>145</v>
       </c>
       <c r="B21" t="s">
-        <v>115</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B22" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B23" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B24" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B25" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B26" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B27" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B28" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B29" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B30" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B31" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>137</v>
+        <v>55</v>
       </c>
       <c r="B32" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B33" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B34" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B35" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>63</v>
+        <v>137</v>
       </c>
       <c r="B36" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B37" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>138</v>
+        <v>61</v>
       </c>
       <c r="B38" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>133</v>
+        <v>62</v>
       </c>
       <c r="B39" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>134</v>
+        <v>63</v>
       </c>
       <c r="B40" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>9</v>
+        <v>64</v>
       </c>
       <c r="B41" t="s">
-        <v>81</v>
+        <v>131</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>12</v>
+        <v>138</v>
       </c>
       <c r="B42" t="s">
-        <v>82</v>
+        <v>139</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>14</v>
+        <v>133</v>
       </c>
       <c r="B43" t="s">
-        <v>83</v>
+        <v>136</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>10</v>
+        <v>134</v>
       </c>
       <c r="B44" t="s">
-        <v>84</v>
+        <v>135</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B45" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B46" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B47" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B48" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B49" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B50" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B51" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B52" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B53" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B54" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B55" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B56" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B57" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B58" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B59" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B60" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B61" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B62" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B63" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B64" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B65" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B66" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B67" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B68" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B69" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>36</v>
+      </c>
+      <c r="B70" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>38</v>
+      </c>
+      <c r="B71" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>34</v>
+      </c>
+      <c r="B72" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>35</v>
+      </c>
+      <c r="B73" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>37</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B74" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add new variables ( o1_per_capita and d1_per_capita)
</commit_message>
<xml_diff>
--- a/docs/RealTimeVariables.xlsx
+++ b/docs/RealTimeVariables.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="152">
   <si>
     <t>pf</t>
   </si>
@@ -463,6 +463,18 @@
   </si>
   <si>
     <t>ردیف</t>
+  </si>
+  <si>
+    <t>o1_per_capita</t>
+  </si>
+  <si>
+    <t>d1_per_capita</t>
+  </si>
+  <si>
+    <t>سرانه صف اول خرید به میلیون تومان</t>
+  </si>
+  <si>
+    <t>سرانه صف اول فروش به میلیون تومان</t>
   </si>
 </sst>
 </file>
@@ -809,10 +821,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C74"/>
+  <dimension ref="A1:C76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,7 +870,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A67" si="0">A3+1</f>
+        <f t="shared" ref="A4:A69" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -1354,10 +1366,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>9</v>
+        <v>149</v>
       </c>
       <c r="C45" t="s">
-        <v>81</v>
+        <v>150</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1366,10 +1378,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>12</v>
+        <v>148</v>
       </c>
       <c r="C46" t="s">
-        <v>82</v>
+        <v>151</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1378,10 +1390,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C47" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1390,10 +1402,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C48" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1402,10 +1414,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C49" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1414,10 +1426,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C50" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1426,10 +1438,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C51" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1438,10 +1450,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C52" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1450,10 +1462,10 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C53" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1462,10 +1474,10 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C54" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1474,10 +1486,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C55" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1486,10 +1498,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C56" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1498,10 +1510,10 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C57" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1510,10 +1522,10 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C58" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1522,10 +1534,10 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C59" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1534,10 +1546,10 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C60" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1546,10 +1558,10 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C61" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -1558,10 +1570,10 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C62" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1570,10 +1582,10 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C63" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -1582,10 +1594,10 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C64" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1594,10 +1606,10 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C65" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1606,10 +1618,10 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C66" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -1618,46 +1630,46 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C67" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
-        <f t="shared" ref="A68:A74" si="1">A67+1</f>
+        <f t="shared" si="0"/>
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C68" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C69" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="A70:A76" si="1">A69+1</f>
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C70" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -1666,10 +1678,10 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C71" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -1678,10 +1690,10 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C72" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -1690,10 +1702,10 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C73" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -1702,9 +1714,33 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
+        <v>34</v>
+      </c>
+      <c r="C74" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>35</v>
+      </c>
+      <c r="C75" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
         <v>37</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C76" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>